<commit_message>
fix fading chord problem
</commit_message>
<xml_diff>
--- a/data/stats.xlsx
+++ b/data/stats.xlsx
@@ -1687,8 +1687,8 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="69134592"/>
-        <c:axId val="69210496"/>
+        <c:axId val="223914624"/>
+        <c:axId val="223970432"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -2148,11 +2148,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="105907328"/>
-        <c:axId val="73095808"/>
+        <c:axId val="223983488"/>
+        <c:axId val="223972736"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="69134592"/>
+        <c:axId val="223914624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2187,14 +2187,14 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="69210496"/>
+        <c:crossAx val="223970432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="69210496"/>
+        <c:axId val="223970432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2221,7 +2221,7 @@
         </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69134592"/>
+        <c:crossAx val="223914624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -2248,7 +2248,7 @@
         </c:dispUnits>
       </c:valAx>
       <c:valAx>
-        <c:axId val="73095808"/>
+        <c:axId val="223972736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2278,7 +2278,7 @@
         </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105907328"/>
+        <c:crossAx val="223983488"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -2305,14 +2305,15 @@
         </c:dispUnits>
       </c:valAx>
       <c:catAx>
-        <c:axId val="105907328"/>
+        <c:axId val="223983488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="73095808"/>
+        <c:crossAx val="223972736"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -2324,9 +2325,9 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.73468699529357728"/>
+          <c:x val="0.7346869952935775"/>
           <c:y val="0.22709867977968062"/>
-          <c:w val="0.26531315051135851"/>
+          <c:w val="0.26531315051135845"/>
           <c:h val="0.26994009410763331"/>
         </c:manualLayout>
       </c:layout>
@@ -2336,7 +2337,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3123,8 +3124,8 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="71574272"/>
-        <c:axId val="71576576"/>
+        <c:axId val="224057984"/>
+        <c:axId val="81347328"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -3878,11 +3879,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="72762880"/>
-        <c:axId val="71616384"/>
+        <c:axId val="81360384"/>
+        <c:axId val="81349632"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="71574272"/>
+        <c:axId val="224057984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3917,14 +3918,14 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71576576"/>
+        <c:crossAx val="81347328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="71576576"/>
+        <c:axId val="81347328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3951,7 +3952,7 @@
         </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71574272"/>
+        <c:crossAx val="224057984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -3978,7 +3979,7 @@
         </c:dispUnits>
       </c:valAx>
       <c:valAx>
-        <c:axId val="71616384"/>
+        <c:axId val="81349632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4008,7 +4009,7 @@
         </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72762880"/>
+        <c:crossAx val="81360384"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -4035,14 +4036,14 @@
         </c:dispUnits>
       </c:valAx>
       <c:catAx>
-        <c:axId val="72762880"/>
+        <c:axId val="81360384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="71616384"/>
+        <c:crossAx val="81349632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4055,7 +4056,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.73468699529357773"/>
+          <c:x val="0.73468699529357784"/>
           <c:y val="0.22709867977968062"/>
           <c:w val="0.11059830413135645"/>
           <c:h val="9.7613546789601893E-2"/>
@@ -4067,7 +4068,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4115,10 +4116,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="9.7645963897369972E-2"/>
-          <c:y val="0.20106532138028202"/>
-          <c:w val="0.81321147356580425"/>
-          <c:h val="0.55296019815704855"/>
+          <c:x val="9.764596389737E-2"/>
+          <c:y val="0.20106532138028205"/>
+          <c:w val="0.81321147356580437"/>
+          <c:h val="0.55296019815704844"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -4146,163 +4147,163 @@
               <c:strCache>
                 <c:ptCount val="53"/>
                 <c:pt idx="0">
+                  <c:v>Alaska</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>California</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Texas</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Florida</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>New York</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>North Dakota</c:v>
-                </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
+                  <c:v>Virginia</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Illinois</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>North Carolina</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>Pennsylvania</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="9">
                   <c:v>Michigan</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="10">
+                  <c:v>Colorado</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Georgia</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Ohio</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>Arizona</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>Alabama</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Hawaii</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Virginia</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Florida</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Nebraska</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>South Dakota</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Mississippi</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>West Virginia</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Massachusetts</c:v>
-                </c:pt>
                 <c:pt idx="14">
-                  <c:v>Indiana</c:v>
+                  <c:v>Tennessee</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>Colorado</c:v>
+                  <c:v>Minnesota</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>Washington</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Kentucky</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>Missouri</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Oklahoma</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>Utah</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>New Jersey</c:v>
                 </c:pt>
                 <c:pt idx="20">
+                  <c:v>Nevada</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Massachusetts</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Indiana</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Utah</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Oregon</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>South Carolina</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>Hawaii</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>Louisiana</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>Wisconsin</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>Maryland</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>Oklahoma</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>Connecticut</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>Nebraska</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>Alabama</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>Iowa</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>New Mexico</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>Puerto Rico</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>Mississippi</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>Montana</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>Arkansas</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>Rhode Island</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>Idaho</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>Maine</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>New Hampshire</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>North Dakota</c:v>
+                </c:pt>
+                <c:pt idx="45">
                   <c:v>Kansas</c:v>
                 </c:pt>
-                <c:pt idx="21">
-                  <c:v>Iowa</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>Maine</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>Puerto Rico</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>Kentucky</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>Washington</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>U.S. Virgin Islands</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>Alaska</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>Tennessee</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>Montana</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>Rhode Island</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>New Mexico</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>Illinois</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>Connecticut</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>California</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>Wisconsin</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>Georgia</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>Texas</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>Arkansas</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>South Carolina</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>Ohio</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>Louisiana</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>Nevada</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>Maryland</c:v>
-                </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="46">
+                  <c:v>South Dakota</c:v>
+                </c:pt>
+                <c:pt idx="47">
                   <c:v>Wyoming</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>Oregon</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>Minnesota</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>Idaho</c:v>
                 </c:pt>
                 <c:pt idx="48">
                   <c:v>Vermont</c:v>
                 </c:pt>
                 <c:pt idx="49">
+                  <c:v>West Virginia</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>U.S. Virgin Islands</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>U.S. Pacific Trust Territories and Possessions</c:v>
+                </c:pt>
+                <c:pt idx="52">
                   <c:v>Delaware</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>U.S. Pacific Trust Territories and Possessions</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>New Hampshire</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>North Carolina</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4311,166 +4312,166 @@
             <c:numRef>
               <c:f>state!$C$2:$C$54</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="53"/>
-                <c:pt idx="0" formatCode="#,##0">
+                <c:pt idx="0">
+                  <c:v>19495</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10444</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10287</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9907</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>7222</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="5">
+                  <c:v>5525</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5497</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4539</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4470</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3981</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3620</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3574</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3487</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3313</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3243</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3035</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3008</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2782</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2551</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2381</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2288</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2141</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1911</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1884</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1752</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1705</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1656</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1550</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1423</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1223</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1041</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1009</c:v>
+                </c:pt>
+                <c:pt idx="33" formatCode="General">
+                  <c:v>922</c:v>
+                </c:pt>
+                <c:pt idx="34" formatCode="General">
+                  <c:v>867</c:v>
+                </c:pt>
+                <c:pt idx="35" formatCode="General">
+                  <c:v>829</c:v>
+                </c:pt>
+                <c:pt idx="36" formatCode="General">
+                  <c:v>795</c:v>
+                </c:pt>
+                <c:pt idx="37" formatCode="General">
+                  <c:v>792</c:v>
+                </c:pt>
+                <c:pt idx="38" formatCode="General">
+                  <c:v>769</c:v>
+                </c:pt>
+                <c:pt idx="39" formatCode="General">
+                  <c:v>721</c:v>
+                </c:pt>
+                <c:pt idx="40" formatCode="General">
+                  <c:v>690</c:v>
+                </c:pt>
+                <c:pt idx="41" formatCode="General">
+                  <c:v>653</c:v>
+                </c:pt>
+                <c:pt idx="42" formatCode="General">
+                  <c:v>620</c:v>
+                </c:pt>
+                <c:pt idx="43" formatCode="General">
+                  <c:v>581</c:v>
+                </c:pt>
+                <c:pt idx="44" formatCode="General">
                   <c:v>535</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="#,##0">
-                  <c:v>4539</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="#,##0">
-                  <c:v>4470</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="#,##0">
-                  <c:v>3487</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>922</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="#,##0">
-                  <c:v>1705</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="#,##0">
-                  <c:v>5525</c:v>
-                </c:pt>
-                <c:pt idx="8" formatCode="#,##0">
-                  <c:v>9907</c:v>
-                </c:pt>
-                <c:pt idx="9" formatCode="#,##0">
-                  <c:v>1009</c:v>
-                </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="45" formatCode="General">
+                  <c:v>523</c:v>
+                </c:pt>
+                <c:pt idx="46" formatCode="General">
                   <c:v>421</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>792</c:v>
-                </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="47" formatCode="General">
+                  <c:v>352</c:v>
+                </c:pt>
+                <c:pt idx="48" formatCode="General">
+                  <c:v>306</c:v>
+                </c:pt>
+                <c:pt idx="49" formatCode="General">
                   <c:v>273</c:v>
                 </c:pt>
-                <c:pt idx="13" formatCode="#,##0">
-                  <c:v>2288</c:v>
-                </c:pt>
-                <c:pt idx="14" formatCode="#,##0">
-                  <c:v>2141</c:v>
-                </c:pt>
-                <c:pt idx="15" formatCode="#,##0">
-                  <c:v>3981</c:v>
-                </c:pt>
-                <c:pt idx="16" formatCode="#,##0">
-                  <c:v>2782</c:v>
-                </c:pt>
-                <c:pt idx="17" formatCode="#,##0">
-                  <c:v>1223</c:v>
-                </c:pt>
-                <c:pt idx="18" formatCode="#,##0">
-                  <c:v>1911</c:v>
-                </c:pt>
-                <c:pt idx="19" formatCode="#,##0">
-                  <c:v>2551</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>523</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>867</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>620</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>795</c:v>
-                </c:pt>
-                <c:pt idx="24" formatCode="#,##0">
-                  <c:v>3008</c:v>
-                </c:pt>
-                <c:pt idx="25" formatCode="#,##0">
-                  <c:v>3035</c:v>
-                </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="50" formatCode="General">
                   <c:v>254</c:v>
                 </c:pt>
-                <c:pt idx="27" formatCode="#,##0">
-                  <c:v>19495</c:v>
-                </c:pt>
-                <c:pt idx="28" formatCode="#,##0">
-                  <c:v>3313</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>769</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>690</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>829</c:v>
-                </c:pt>
-                <c:pt idx="32" formatCode="#,##0">
-                  <c:v>5497</c:v>
-                </c:pt>
-                <c:pt idx="33" formatCode="#,##0">
-                  <c:v>1041</c:v>
-                </c:pt>
-                <c:pt idx="34" formatCode="#,##0">
-                  <c:v>10444</c:v>
-                </c:pt>
-                <c:pt idx="35" formatCode="#,##0">
-                  <c:v>1550</c:v>
-                </c:pt>
-                <c:pt idx="36" formatCode="#,##0">
-                  <c:v>3620</c:v>
-                </c:pt>
-                <c:pt idx="37" formatCode="#,##0">
-                  <c:v>10287</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>721</c:v>
-                </c:pt>
-                <c:pt idx="39" formatCode="#,##0">
-                  <c:v>1752</c:v>
-                </c:pt>
-                <c:pt idx="40" formatCode="#,##0">
-                  <c:v>3574</c:v>
-                </c:pt>
-                <c:pt idx="41" formatCode="#,##0">
-                  <c:v>1656</c:v>
-                </c:pt>
-                <c:pt idx="42" formatCode="#,##0">
-                  <c:v>2381</c:v>
-                </c:pt>
-                <c:pt idx="43" formatCode="#,##0">
-                  <c:v>1423</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>352</c:v>
-                </c:pt>
-                <c:pt idx="45" formatCode="#,##0">
-                  <c:v>1884</c:v>
-                </c:pt>
-                <c:pt idx="46" formatCode="#,##0">
-                  <c:v>3243</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>653</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>306</c:v>
-                </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="51" formatCode="General">
+                  <c:v>177</c:v>
+                </c:pt>
+                <c:pt idx="52" formatCode="General">
                   <c:v>59</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>177</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>581</c:v>
-                </c:pt>
-                <c:pt idx="52" formatCode="#,##0">
-                  <c:v>5000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4499,163 +4500,163 @@
               <c:strCache>
                 <c:ptCount val="53"/>
                 <c:pt idx="0">
+                  <c:v>Alaska</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>California</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Texas</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Florida</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>New York</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>North Dakota</c:v>
-                </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
+                  <c:v>Virginia</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Illinois</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>North Carolina</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>Pennsylvania</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="9">
                   <c:v>Michigan</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="10">
+                  <c:v>Colorado</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Georgia</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Ohio</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>Arizona</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>Alabama</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Hawaii</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Virginia</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Florida</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Nebraska</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>South Dakota</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Mississippi</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>West Virginia</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Massachusetts</c:v>
-                </c:pt>
                 <c:pt idx="14">
-                  <c:v>Indiana</c:v>
+                  <c:v>Tennessee</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>Colorado</c:v>
+                  <c:v>Minnesota</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>Washington</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Kentucky</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>Missouri</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Oklahoma</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>Utah</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>New Jersey</c:v>
                 </c:pt>
                 <c:pt idx="20">
+                  <c:v>Nevada</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Massachusetts</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Indiana</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Utah</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Oregon</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>South Carolina</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>Hawaii</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>Louisiana</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>Wisconsin</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>Maryland</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>Oklahoma</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>Connecticut</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>Nebraska</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>Alabama</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>Iowa</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>New Mexico</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>Puerto Rico</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>Mississippi</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>Montana</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>Arkansas</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>Rhode Island</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>Idaho</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>Maine</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>New Hampshire</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>North Dakota</c:v>
+                </c:pt>
+                <c:pt idx="45">
                   <c:v>Kansas</c:v>
                 </c:pt>
-                <c:pt idx="21">
-                  <c:v>Iowa</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>Maine</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>Puerto Rico</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>Kentucky</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>Washington</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>U.S. Virgin Islands</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>Alaska</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>Tennessee</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>Montana</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>Rhode Island</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>New Mexico</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>Illinois</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>Connecticut</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>California</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>Wisconsin</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>Georgia</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>Texas</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>Arkansas</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>South Carolina</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>Ohio</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>Louisiana</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>Nevada</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>Maryland</c:v>
-                </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="46">
+                  <c:v>South Dakota</c:v>
+                </c:pt>
+                <c:pt idx="47">
                   <c:v>Wyoming</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>Oregon</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>Minnesota</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>Idaho</c:v>
                 </c:pt>
                 <c:pt idx="48">
                   <c:v>Vermont</c:v>
                 </c:pt>
                 <c:pt idx="49">
+                  <c:v>West Virginia</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>U.S. Virgin Islands</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>U.S. Pacific Trust Territories and Possessions</c:v>
+                </c:pt>
+                <c:pt idx="52">
                   <c:v>Delaware</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>U.S. Pacific Trust Territories and Possessions</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>New Hampshire</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>North Carolina</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4664,174 +4665,174 @@
             <c:numRef>
               <c:f>state!$D$2:$D$54</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="53"/>
-                <c:pt idx="0" formatCode="#,##0">
+                <c:pt idx="0">
+                  <c:v>19467</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10469</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10254</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10194</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>7270</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="5">
+                  <c:v>5551</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5468</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5069</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4520</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4458</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3985</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3684</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3559</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3540</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3327</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3209</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3011</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2924</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2737</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2545</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2369</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2289</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2072</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1887</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1884</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1746</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1592</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1669</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1557</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1415</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1173</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1043</c:v>
+                </c:pt>
+                <c:pt idx="32" formatCode="General">
+                  <c:v>976</c:v>
+                </c:pt>
+                <c:pt idx="33" formatCode="General">
+                  <c:v>891</c:v>
+                </c:pt>
+                <c:pt idx="34" formatCode="General">
+                  <c:v>871</c:v>
+                </c:pt>
+                <c:pt idx="35" formatCode="General">
+                  <c:v>845</c:v>
+                </c:pt>
+                <c:pt idx="36" formatCode="General">
+                  <c:v>807</c:v>
+                </c:pt>
+                <c:pt idx="37" formatCode="General">
+                  <c:v>776</c:v>
+                </c:pt>
+                <c:pt idx="38" formatCode="General">
+                  <c:v>805</c:v>
+                </c:pt>
+                <c:pt idx="39" formatCode="General">
+                  <c:v>726</c:v>
+                </c:pt>
+                <c:pt idx="40" formatCode="General">
+                  <c:v>716</c:v>
+                </c:pt>
+                <c:pt idx="41" formatCode="General">
+                  <c:v>614</c:v>
+                </c:pt>
+                <c:pt idx="42" formatCode="General">
+                  <c:v>659</c:v>
+                </c:pt>
+                <c:pt idx="43" formatCode="General">
+                  <c:v>558</c:v>
+                </c:pt>
+                <c:pt idx="44" formatCode="General">
                   <c:v>531</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="#,##0">
-                  <c:v>4520</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="#,##0">
-                  <c:v>4458</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="#,##0">
-                  <c:v>3540</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>891</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="#,##0">
-                  <c:v>1592</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="#,##0">
-                  <c:v>5551</c:v>
-                </c:pt>
-                <c:pt idx="8" formatCode="#,##0">
-                  <c:v>10194</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>976</c:v>
-                </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="45" formatCode="General">
+                  <c:v>522</c:v>
+                </c:pt>
+                <c:pt idx="46" formatCode="General">
                   <c:v>417</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>776</c:v>
-                </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="47" formatCode="General">
+                  <c:v>339</c:v>
+                </c:pt>
+                <c:pt idx="48" formatCode="General">
+                  <c:v>316</c:v>
+                </c:pt>
+                <c:pt idx="49" formatCode="General">
                   <c:v>281</c:v>
                 </c:pt>
-                <c:pt idx="13" formatCode="#,##0">
-                  <c:v>2289</c:v>
-                </c:pt>
-                <c:pt idx="14" formatCode="#,##0">
-                  <c:v>2072</c:v>
-                </c:pt>
-                <c:pt idx="15" formatCode="#,##0">
-                  <c:v>3985</c:v>
-                </c:pt>
-                <c:pt idx="16" formatCode="#,##0">
-                  <c:v>2737</c:v>
-                </c:pt>
-                <c:pt idx="17" formatCode="#,##0">
-                  <c:v>1173</c:v>
-                </c:pt>
-                <c:pt idx="18" formatCode="#,##0">
-                  <c:v>1887</c:v>
-                </c:pt>
-                <c:pt idx="19" formatCode="#,##0">
-                  <c:v>2545</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>522</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>871</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>659</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>807</c:v>
-                </c:pt>
-                <c:pt idx="24" formatCode="#,##0">
-                  <c:v>2924</c:v>
-                </c:pt>
-                <c:pt idx="25" formatCode="#,##0">
-                  <c:v>3011</c:v>
-                </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="50" formatCode="General">
                   <c:v>288</c:v>
                 </c:pt>
-                <c:pt idx="27" formatCode="#,##0">
-                  <c:v>19467</c:v>
-                </c:pt>
-                <c:pt idx="28" formatCode="#,##0">
-                  <c:v>3327</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>805</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>716</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>845</c:v>
-                </c:pt>
-                <c:pt idx="32" formatCode="#,##0">
-                  <c:v>5468</c:v>
-                </c:pt>
-                <c:pt idx="33" formatCode="#,##0">
-                  <c:v>1043</c:v>
-                </c:pt>
-                <c:pt idx="34" formatCode="#,##0">
-                  <c:v>10469</c:v>
-                </c:pt>
-                <c:pt idx="35" formatCode="#,##0">
-                  <c:v>1557</c:v>
-                </c:pt>
-                <c:pt idx="36" formatCode="#,##0">
-                  <c:v>3684</c:v>
-                </c:pt>
-                <c:pt idx="37" formatCode="#,##0">
-                  <c:v>10254</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>726</c:v>
-                </c:pt>
-                <c:pt idx="39" formatCode="#,##0">
-                  <c:v>1746</c:v>
-                </c:pt>
-                <c:pt idx="40" formatCode="#,##0">
-                  <c:v>3559</c:v>
-                </c:pt>
-                <c:pt idx="41" formatCode="#,##0">
-                  <c:v>1669</c:v>
-                </c:pt>
-                <c:pt idx="42" formatCode="#,##0">
-                  <c:v>2369</c:v>
-                </c:pt>
-                <c:pt idx="43" formatCode="#,##0">
-                  <c:v>1415</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>339</c:v>
-                </c:pt>
-                <c:pt idx="45" formatCode="#,##0">
-                  <c:v>1884</c:v>
-                </c:pt>
-                <c:pt idx="46" formatCode="#,##0">
-                  <c:v>3209</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>614</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>316</c:v>
-                </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="51" formatCode="General">
+                  <c:v>157</c:v>
+                </c:pt>
+                <c:pt idx="52" formatCode="General">
                   <c:v>51</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>157</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>558</c:v>
-                </c:pt>
-                <c:pt idx="52" formatCode="#,##0">
-                  <c:v>5069</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="104672640"/>
-        <c:axId val="104674816"/>
+        <c:axId val="156355968"/>
+        <c:axId val="79541376"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -4858,163 +4859,163 @@
               <c:strCache>
                 <c:ptCount val="53"/>
                 <c:pt idx="0">
+                  <c:v>Alaska</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>California</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Texas</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Florida</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>New York</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>North Dakota</c:v>
-                </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
+                  <c:v>Virginia</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Illinois</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>North Carolina</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>Pennsylvania</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="9">
                   <c:v>Michigan</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="10">
+                  <c:v>Colorado</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Georgia</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Ohio</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>Arizona</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>Alabama</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Hawaii</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Virginia</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Florida</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Nebraska</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>South Dakota</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Mississippi</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>West Virginia</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Massachusetts</c:v>
-                </c:pt>
                 <c:pt idx="14">
-                  <c:v>Indiana</c:v>
+                  <c:v>Tennessee</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>Colorado</c:v>
+                  <c:v>Minnesota</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>Washington</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Kentucky</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>Missouri</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Oklahoma</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>Utah</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>New Jersey</c:v>
                 </c:pt>
                 <c:pt idx="20">
+                  <c:v>Nevada</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Massachusetts</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Indiana</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Utah</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Oregon</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>South Carolina</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>Hawaii</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>Louisiana</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>Wisconsin</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>Maryland</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>Oklahoma</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>Connecticut</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>Nebraska</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>Alabama</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>Iowa</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>New Mexico</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>Puerto Rico</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>Mississippi</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>Montana</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>Arkansas</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>Rhode Island</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>Idaho</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>Maine</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>New Hampshire</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>North Dakota</c:v>
+                </c:pt>
+                <c:pt idx="45">
                   <c:v>Kansas</c:v>
                 </c:pt>
-                <c:pt idx="21">
-                  <c:v>Iowa</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>Maine</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>Puerto Rico</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>Kentucky</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>Washington</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>U.S. Virgin Islands</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>Alaska</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>Tennessee</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>Montana</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>Rhode Island</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>New Mexico</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>Illinois</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>Connecticut</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>California</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>Wisconsin</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>Georgia</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>Texas</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>Arkansas</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>South Carolina</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>Ohio</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>Louisiana</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>Nevada</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>Maryland</c:v>
-                </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="46">
+                  <c:v>South Dakota</c:v>
+                </c:pt>
+                <c:pt idx="47">
                   <c:v>Wyoming</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>Oregon</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>Minnesota</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>Idaho</c:v>
                 </c:pt>
                 <c:pt idx="48">
                   <c:v>Vermont</c:v>
                 </c:pt>
                 <c:pt idx="49">
+                  <c:v>West Virginia</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>U.S. Virgin Islands</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>U.S. Pacific Trust Territories and Possessions</c:v>
+                </c:pt>
+                <c:pt idx="52">
                   <c:v>Delaware</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>U.S. Pacific Trust Territories and Possessions</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>New Hampshire</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>North Carolina</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5026,174 +5027,174 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="53"/>
                 <c:pt idx="0">
+                  <c:v>2567297</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1348014</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1035328</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13024532</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>44974952</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>38344087</c:v>
-                </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
+                  <c:v>15416489</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1684357</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>69472</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>35066219</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="9">
                   <c:v>24717253</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="10">
+                  <c:v>7821506</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1052804</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>971035</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>22420198</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>18934616</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>15518404</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>15416489</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>13024532</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>11980309</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11973766</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>10535011</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>10467235</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>9593764</c:v>
-                </c:pt>
                 <c:pt idx="14">
-                  <c:v>9409376</c:v>
+                  <c:v>2561628</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7821506</c:v>
+                  <c:v>506842</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>2925502</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3580100</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>7754252</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>7356054</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>6685367</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>6185185</c:v>
                 </c:pt>
                 <c:pt idx="20">
+                  <c:v>616387</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9593764</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9409376</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>6685367</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>568405</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1013971</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>15518404</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>721820</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1324869</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>612441</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>7356054</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1425502</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>11980309</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>18934616</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>5225836</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1892254</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>4936285</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>10535011</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2540308</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1024124</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2262803</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>454533</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4945762</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>164616</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>38344087</c:v>
+                </c:pt>
+                <c:pt idx="45">
                   <c:v>5912447</c:v>
                 </c:pt>
-                <c:pt idx="21">
-                  <c:v>5225836</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>4945762</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>4936285</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>3580100</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>2925502</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>2822856</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>2567297</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>2561628</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>2540308</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>2262803</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>1892254</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>1684357</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>1425502</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>1348014</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>1324869</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>1052804</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>1035328</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>1024124</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>1013971</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>971035</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>721820</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>616387</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>612441</c:v>
-                </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="46">
+                  <c:v>11973766</c:v>
+                </c:pt>
+                <c:pt idx="47">
                   <c:v>611595</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>568405</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>506842</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>454533</c:v>
                 </c:pt>
                 <c:pt idx="48">
                   <c:v>346782</c:v>
                 </c:pt>
                 <c:pt idx="49">
+                  <c:v>10467235</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2822856</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>228901</c:v>
+                </c:pt>
+                <c:pt idx="52">
                   <c:v>312989</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>228901</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>164616</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>69472</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="266763264"/>
-        <c:axId val="266760960"/>
+        <c:axId val="79550336"/>
+        <c:axId val="79543680"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="104672640"/>
+        <c:axId val="156355968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5218,14 +5219,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104674816"/>
+        <c:crossAx val="79541376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="104674816"/>
+        <c:axId val="79541376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5252,7 +5253,7 @@
         </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104672640"/>
+        <c:crossAx val="156355968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1000"/>
@@ -5261,7 +5262,7 @@
         </c:dispUnits>
       </c:valAx>
       <c:valAx>
-        <c:axId val="266760960"/>
+        <c:axId val="79543680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5287,7 +5288,7 @@
         </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="266763264"/>
+        <c:crossAx val="79550336"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -5295,14 +5296,15 @@
         </c:dispUnits>
       </c:valAx>
       <c:catAx>
-        <c:axId val="266763264"/>
+        <c:axId val="79550336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="266760960"/>
+        <c:crossAx val="79543680"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -5316,7 +5318,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7413,8 +7415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B54" sqref="B2:B54"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25"/>
@@ -7434,326 +7436,326 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="13" t="s">
-        <v>304</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>305</v>
-      </c>
-      <c r="C2" s="8">
-        <v>7222</v>
-      </c>
-      <c r="D2" s="8">
-        <v>7270</v>
+      <c r="A2" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="C2" s="9">
+        <v>19495</v>
+      </c>
+      <c r="D2" s="9">
+        <v>19467</v>
       </c>
       <c r="E2" s="9">
-        <v>44974952</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="21">
-      <c r="A3" s="13" t="s">
-        <v>292</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>293</v>
-      </c>
-      <c r="C3" s="7">
-        <v>535</v>
-      </c>
-      <c r="D3" s="7">
-        <v>531</v>
-      </c>
-      <c r="E3" s="9">
-        <v>38344087</v>
+        <v>2567297</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="12" t="s">
+        <v>249</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="C3" s="9">
+        <v>10444</v>
+      </c>
+      <c r="D3" s="9">
+        <v>10469</v>
+      </c>
+      <c r="E3" s="8">
+        <v>1348014</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="13" t="s">
-        <v>312</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>313</v>
-      </c>
-      <c r="C4" s="8">
-        <v>4539</v>
-      </c>
-      <c r="D4" s="8">
-        <v>4520</v>
+      <c r="A4" s="12" t="s">
+        <v>326</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="C4" s="9">
+        <v>10287</v>
+      </c>
+      <c r="D4" s="9">
+        <v>10254</v>
       </c>
       <c r="E4" s="9">
-        <v>35066219</v>
+        <v>1035328</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="13" t="s">
-        <v>281</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>282</v>
-      </c>
-      <c r="C5" s="8">
-        <v>4470</v>
-      </c>
-      <c r="D5" s="8">
-        <v>4458</v>
+      <c r="A5" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="C5" s="9">
+        <v>9907</v>
+      </c>
+      <c r="D5" s="9">
+        <v>10194</v>
       </c>
       <c r="E5" s="8">
-        <v>24717253</v>
+        <v>13024532</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="13" t="s">
+        <v>304</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="C6" s="8">
+        <v>7222</v>
+      </c>
+      <c r="D6" s="8">
+        <v>7270</v>
+      </c>
+      <c r="E6" s="9">
+        <v>44974952</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="12" t="s">
+        <v>330</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="C7" s="9">
+        <v>5525</v>
+      </c>
+      <c r="D7" s="9">
+        <v>5551</v>
+      </c>
+      <c r="E7" s="8">
+        <v>15416489</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="13" t="s">
+        <v>266</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="C8" s="8">
+        <v>5497</v>
+      </c>
+      <c r="D8" s="8">
+        <v>5468</v>
+      </c>
+      <c r="E8" s="9">
+        <v>1684357</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="21">
+      <c r="A9" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="C9" s="9">
+        <v>5000</v>
+      </c>
+      <c r="D9" s="9">
+        <v>5069</v>
+      </c>
+      <c r="E9" s="8">
+        <v>69472</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="13" t="s">
+        <v>312</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="C10" s="8">
+        <v>4539</v>
+      </c>
+      <c r="D10" s="8">
+        <v>4520</v>
+      </c>
+      <c r="E10" s="9">
+        <v>35066219</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="C11" s="8">
+        <v>4470</v>
+      </c>
+      <c r="D11" s="8">
+        <v>4458</v>
+      </c>
+      <c r="E11" s="8">
+        <v>24717253</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="C12" s="8">
+        <v>3981</v>
+      </c>
+      <c r="D12" s="8">
+        <v>3985</v>
+      </c>
+      <c r="E12" s="9">
+        <v>7821506</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="C13" s="8">
+        <v>3620</v>
+      </c>
+      <c r="D13" s="8">
+        <v>3684</v>
+      </c>
+      <c r="E13" s="8">
+        <v>1052804</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="12" t="s">
+        <v>306</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="C14" s="9">
+        <v>3574</v>
+      </c>
+      <c r="D14" s="9">
+        <v>3559</v>
+      </c>
+      <c r="E14" s="9">
+        <v>971035</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="13" t="s">
         <v>247</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B15" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C15" s="8">
         <v>3487</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D15" s="8">
         <v>3540</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E15" s="8">
         <v>22420198</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="13" t="s">
-        <v>243</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>244</v>
-      </c>
-      <c r="C7" s="7">
-        <v>922</v>
-      </c>
-      <c r="D7" s="7">
-        <v>891</v>
-      </c>
-      <c r="E7" s="8">
-        <v>18934616</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="12" t="s">
-        <v>260</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>261</v>
-      </c>
-      <c r="C8" s="9">
-        <v>1705</v>
-      </c>
-      <c r="D8" s="9">
-        <v>1592</v>
-      </c>
-      <c r="E8" s="9">
-        <v>15518404</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="12" t="s">
-        <v>330</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>331</v>
-      </c>
-      <c r="C9" s="9">
-        <v>5525</v>
-      </c>
-      <c r="D9" s="9">
-        <v>5551</v>
-      </c>
-      <c r="E9" s="8">
-        <v>15416489</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="C10" s="9">
-        <v>9907</v>
-      </c>
-      <c r="D10" s="9">
-        <v>10194</v>
-      </c>
-      <c r="E10" s="8">
-        <v>13024532</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="12" t="s">
-        <v>294</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="C11" s="9">
-        <v>1009</v>
-      </c>
-      <c r="D11" s="5">
-        <v>976</v>
-      </c>
-      <c r="E11" s="9">
-        <v>11980309</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="21">
-      <c r="A12" s="13" t="s">
-        <v>320</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>321</v>
-      </c>
-      <c r="C12" s="7">
-        <v>421</v>
-      </c>
-      <c r="D12" s="7">
-        <v>417</v>
-      </c>
-      <c r="E12" s="9">
-        <v>11973766</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="12" t="s">
-        <v>287</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>288</v>
-      </c>
-      <c r="C13" s="5">
-        <v>792</v>
-      </c>
-      <c r="D13" s="5">
-        <v>776</v>
-      </c>
-      <c r="E13" s="8">
-        <v>10535011</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="13" t="s">
-        <v>338</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>339</v>
-      </c>
-      <c r="C14" s="7">
-        <v>273</v>
-      </c>
-      <c r="D14" s="7">
-        <v>281</v>
-      </c>
-      <c r="E14" s="8">
-        <v>10467235</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="21">
-      <c r="A15" s="12" t="s">
-        <v>275</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="C15" s="9">
-        <v>2288</v>
-      </c>
-      <c r="D15" s="9">
-        <v>2289</v>
-      </c>
-      <c r="E15" s="8">
-        <v>9593764</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="12" t="s">
-        <v>268</v>
+        <v>322</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>269</v>
+        <v>323</v>
       </c>
       <c r="C16" s="9">
-        <v>2141</v>
+        <v>3313</v>
       </c>
       <c r="D16" s="9">
-        <v>2072</v>
+        <v>3327</v>
       </c>
       <c r="E16" s="9">
-        <v>9409376</v>
+        <v>2561628</v>
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="13" t="s">
-        <v>251</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>252</v>
-      </c>
-      <c r="C17" s="8">
-        <v>3981</v>
-      </c>
-      <c r="D17" s="8">
-        <v>3985</v>
-      </c>
-      <c r="E17" s="9">
-        <v>7821506</v>
+      <c r="A17" s="12" t="s">
+        <v>283</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="C17" s="9">
+        <v>3243</v>
+      </c>
+      <c r="D17" s="9">
+        <v>3209</v>
+      </c>
+      <c r="E17" s="8">
+        <v>506842</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="13" t="s">
-        <v>285</v>
+        <v>335</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>286</v>
+        <v>336</v>
       </c>
       <c r="C18" s="8">
-        <v>2782</v>
+        <v>3035</v>
       </c>
       <c r="D18" s="8">
-        <v>2737</v>
+        <v>3011</v>
       </c>
       <c r="E18" s="9">
-        <v>7754252</v>
+        <v>2925502</v>
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="13" t="s">
-        <v>308</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>309</v>
-      </c>
-      <c r="C19" s="8">
-        <v>1223</v>
-      </c>
-      <c r="D19" s="8">
-        <v>1173</v>
-      </c>
-      <c r="E19" s="9">
-        <v>7356054</v>
+      <c r="A19" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="C19" s="9">
+        <v>3008</v>
+      </c>
+      <c r="D19" s="9">
+        <v>2924</v>
+      </c>
+      <c r="E19" s="8">
+        <v>3580100</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="13" t="s">
-        <v>328</v>
+        <v>285</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="C20" s="8">
-        <v>1911</v>
+        <v>2782</v>
       </c>
       <c r="D20" s="8">
-        <v>1887</v>
-      </c>
-      <c r="E20" s="8">
-        <v>6685367</v>
+        <v>2737</v>
+      </c>
+      <c r="E20" s="9">
+        <v>7754252</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -7774,479 +7776,479 @@
       </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="13" t="s">
-        <v>150</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="C22" s="7">
-        <v>523</v>
-      </c>
-      <c r="D22" s="7">
-        <v>522</v>
-      </c>
-      <c r="E22" s="8">
-        <v>5912447</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="13" t="s">
-        <v>262</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="C23" s="7">
-        <v>867</v>
-      </c>
-      <c r="D23" s="7">
-        <v>871</v>
-      </c>
-      <c r="E23" s="9">
-        <v>5225836</v>
+      <c r="A22" s="12" t="s">
+        <v>302</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="C22" s="9">
+        <v>2381</v>
+      </c>
+      <c r="D22" s="9">
+        <v>2369</v>
+      </c>
+      <c r="E22" s="9">
+        <v>616387</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="21">
+      <c r="A23" s="12" t="s">
+        <v>275</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="C23" s="9">
+        <v>2288</v>
+      </c>
+      <c r="D23" s="9">
+        <v>2289</v>
+      </c>
+      <c r="E23" s="8">
+        <v>9593764</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="12" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>280</v>
-      </c>
-      <c r="C24" s="5">
-        <v>620</v>
-      </c>
-      <c r="D24" s="5">
-        <v>659</v>
+        <v>269</v>
+      </c>
+      <c r="C24" s="9">
+        <v>2141</v>
+      </c>
+      <c r="D24" s="9">
+        <v>2072</v>
       </c>
       <c r="E24" s="9">
-        <v>4945762</v>
+        <v>9409376</v>
       </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="12" t="s">
-        <v>314</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>315</v>
-      </c>
-      <c r="C25" s="5">
-        <v>795</v>
-      </c>
-      <c r="D25" s="5">
-        <v>807</v>
-      </c>
-      <c r="E25" s="9">
-        <v>4936285</v>
+      <c r="A25" s="13" t="s">
+        <v>328</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>329</v>
+      </c>
+      <c r="C25" s="8">
+        <v>1911</v>
+      </c>
+      <c r="D25" s="8">
+        <v>1887</v>
+      </c>
+      <c r="E25" s="8">
+        <v>6685367</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="12" t="s">
-        <v>271</v>
+        <v>310</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>272</v>
+        <v>311</v>
       </c>
       <c r="C26" s="9">
-        <v>3008</v>
+        <v>1884</v>
       </c>
       <c r="D26" s="9">
-        <v>2924</v>
-      </c>
-      <c r="E26" s="8">
-        <v>3580100</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="13" t="s">
-        <v>335</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>336</v>
-      </c>
-      <c r="C27" s="8">
-        <v>3035</v>
-      </c>
-      <c r="D27" s="8">
-        <v>3011</v>
-      </c>
-      <c r="E27" s="9">
-        <v>2925502</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="21">
-      <c r="A28" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>332</v>
-      </c>
-      <c r="C28" s="7">
-        <v>254</v>
-      </c>
-      <c r="D28" s="7">
-        <v>288</v>
+        <v>1884</v>
+      </c>
+      <c r="E26" s="9">
+        <v>568405</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="21">
+      <c r="A27" s="12" t="s">
+        <v>318</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="C27" s="9">
+        <v>1752</v>
+      </c>
+      <c r="D27" s="9">
+        <v>1746</v>
+      </c>
+      <c r="E27" s="8">
+        <v>1013971</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="12" t="s">
+        <v>260</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="C28" s="9">
+        <v>1705</v>
+      </c>
+      <c r="D28" s="9">
+        <v>1592</v>
       </c>
       <c r="E28" s="9">
-        <v>2822856</v>
+        <v>15518404</v>
       </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="12" t="s">
-        <v>241</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="C29" s="9">
-        <v>19495</v>
-      </c>
-      <c r="D29" s="9">
-        <v>19467</v>
-      </c>
-      <c r="E29" s="9">
-        <v>2567297</v>
+      <c r="A29" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="C29" s="8">
+        <v>1656</v>
+      </c>
+      <c r="D29" s="8">
+        <v>1669</v>
+      </c>
+      <c r="E29" s="8">
+        <v>721820</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="12" t="s">
-        <v>322</v>
+        <v>208</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>323</v>
+        <v>337</v>
       </c>
       <c r="C30" s="9">
-        <v>3313</v>
+        <v>1550</v>
       </c>
       <c r="D30" s="9">
-        <v>3327</v>
+        <v>1557</v>
       </c>
       <c r="E30" s="9">
-        <v>2561628</v>
+        <v>1324869</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="13" t="s">
-        <v>289</v>
+        <v>277</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>290</v>
-      </c>
-      <c r="C31" s="7">
-        <v>769</v>
-      </c>
-      <c r="D31" s="7">
-        <v>805</v>
-      </c>
-      <c r="E31" s="9">
-        <v>2540308</v>
+        <v>278</v>
+      </c>
+      <c r="C31" s="8">
+        <v>1423</v>
+      </c>
+      <c r="D31" s="8">
+        <v>1415</v>
+      </c>
+      <c r="E31" s="8">
+        <v>612441</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="13" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>317</v>
-      </c>
-      <c r="C32" s="7">
-        <v>690</v>
-      </c>
-      <c r="D32" s="7">
-        <v>716</v>
+        <v>309</v>
+      </c>
+      <c r="C32" s="8">
+        <v>1223</v>
+      </c>
+      <c r="D32" s="8">
+        <v>1173</v>
       </c>
       <c r="E32" s="9">
-        <v>2262803</v>
+        <v>7356054</v>
       </c>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="13" t="s">
+      <c r="A33" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="C33" s="9">
+        <v>1041</v>
+      </c>
+      <c r="D33" s="9">
+        <v>1043</v>
+      </c>
+      <c r="E33" s="8">
+        <v>1425502</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="12" t="s">
+        <v>294</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="C34" s="9">
+        <v>1009</v>
+      </c>
+      <c r="D34" s="5">
+        <v>976</v>
+      </c>
+      <c r="E34" s="9">
+        <v>11980309</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="13" t="s">
+        <v>243</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="C35" s="7">
+        <v>922</v>
+      </c>
+      <c r="D35" s="7">
+        <v>891</v>
+      </c>
+      <c r="E35" s="8">
+        <v>18934616</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="13" t="s">
+        <v>262</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="C36" s="7">
+        <v>867</v>
+      </c>
+      <c r="D36" s="7">
+        <v>871</v>
+      </c>
+      <c r="E36" s="9">
+        <v>5225836</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="13" t="s">
         <v>300</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B37" s="6" t="s">
         <v>301</v>
       </c>
-      <c r="C33" s="7">
+      <c r="C37" s="7">
         <v>829</v>
       </c>
-      <c r="D33" s="7">
+      <c r="D37" s="7">
         <v>845</v>
       </c>
-      <c r="E33" s="8">
+      <c r="E37" s="8">
         <v>1892254</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="13" t="s">
-        <v>266</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>267</v>
-      </c>
-      <c r="C34" s="8">
-        <v>5497</v>
-      </c>
-      <c r="D34" s="8">
-        <v>5468</v>
-      </c>
-      <c r="E34" s="9">
-        <v>1684357</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="12" t="s">
-        <v>253</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="C35" s="9">
-        <v>1041</v>
-      </c>
-      <c r="D35" s="9">
-        <v>1043</v>
-      </c>
-      <c r="E35" s="8">
-        <v>1425502</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="12" t="s">
-        <v>249</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="C36" s="9">
-        <v>10444</v>
-      </c>
-      <c r="D36" s="9">
-        <v>10469</v>
-      </c>
-      <c r="E36" s="8">
-        <v>1348014</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="12" t="s">
-        <v>208</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>337</v>
-      </c>
-      <c r="C37" s="9">
-        <v>1550</v>
-      </c>
-      <c r="D37" s="9">
-        <v>1557</v>
-      </c>
-      <c r="E37" s="9">
-        <v>1324869</v>
-      </c>
-    </row>
     <row r="38" spans="1:5">
-      <c r="A38" s="13" t="s">
-        <v>258</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>259</v>
-      </c>
-      <c r="C38" s="8">
-        <v>3620</v>
-      </c>
-      <c r="D38" s="8">
-        <v>3684</v>
-      </c>
-      <c r="E38" s="8">
-        <v>1052804</v>
+      <c r="A38" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="C38" s="5">
+        <v>795</v>
+      </c>
+      <c r="D38" s="5">
+        <v>807</v>
+      </c>
+      <c r="E38" s="9">
+        <v>4936285</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="12" t="s">
-        <v>326</v>
+        <v>287</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>327</v>
-      </c>
-      <c r="C39" s="9">
-        <v>10287</v>
-      </c>
-      <c r="D39" s="9">
-        <v>10254</v>
-      </c>
-      <c r="E39" s="9">
-        <v>1035328</v>
+        <v>288</v>
+      </c>
+      <c r="C39" s="5">
+        <v>792</v>
+      </c>
+      <c r="D39" s="5">
+        <v>776</v>
+      </c>
+      <c r="E39" s="8">
+        <v>10535011</v>
       </c>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="12" t="s">
+      <c r="A40" s="13" t="s">
+        <v>289</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="C40" s="7">
+        <v>769</v>
+      </c>
+      <c r="D40" s="7">
+        <v>805</v>
+      </c>
+      <c r="E40" s="9">
+        <v>2540308</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="12" t="s">
         <v>245</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B41" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="C40" s="5">
+      <c r="C41" s="5">
         <v>721</v>
       </c>
-      <c r="D40" s="5">
+      <c r="D41" s="5">
         <v>726</v>
       </c>
-      <c r="E40" s="8">
+      <c r="E41" s="8">
         <v>1024124</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="21">
-      <c r="A41" s="12" t="s">
-        <v>318</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>319</v>
-      </c>
-      <c r="C41" s="9">
-        <v>1752</v>
-      </c>
-      <c r="D41" s="9">
-        <v>1746</v>
-      </c>
-      <c r="E41" s="8">
-        <v>1013971</v>
-      </c>
-    </row>
     <row r="42" spans="1:5">
-      <c r="A42" s="12" t="s">
-        <v>306</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>307</v>
-      </c>
-      <c r="C42" s="9">
-        <v>3574</v>
-      </c>
-      <c r="D42" s="9">
-        <v>3559</v>
+      <c r="A42" s="13" t="s">
+        <v>316</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="C42" s="7">
+        <v>690</v>
+      </c>
+      <c r="D42" s="7">
+        <v>716</v>
       </c>
       <c r="E42" s="9">
-        <v>971035</v>
+        <v>2262803</v>
       </c>
     </row>
     <row r="43" spans="1:5">
-      <c r="A43" s="13" t="s">
-        <v>273</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>274</v>
-      </c>
-      <c r="C43" s="8">
-        <v>1656</v>
-      </c>
-      <c r="D43" s="8">
-        <v>1669</v>
+      <c r="A43" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="C43" s="5">
+        <v>653</v>
+      </c>
+      <c r="D43" s="5">
+        <v>614</v>
       </c>
       <c r="E43" s="8">
-        <v>721820</v>
+        <v>454533</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="12" t="s">
-        <v>302</v>
+        <v>279</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>303</v>
-      </c>
-      <c r="C44" s="9">
-        <v>2381</v>
-      </c>
-      <c r="D44" s="9">
-        <v>2369</v>
+        <v>280</v>
+      </c>
+      <c r="C44" s="5">
+        <v>620</v>
+      </c>
+      <c r="D44" s="5">
+        <v>659</v>
       </c>
       <c r="E44" s="9">
-        <v>616387</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
+        <v>4945762</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="21">
       <c r="A45" s="13" t="s">
-        <v>277</v>
+        <v>296</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>278</v>
-      </c>
-      <c r="C45" s="8">
-        <v>1423</v>
-      </c>
-      <c r="D45" s="8">
-        <v>1415</v>
+        <v>297</v>
+      </c>
+      <c r="C45" s="7">
+        <v>581</v>
+      </c>
+      <c r="D45" s="7">
+        <v>558</v>
       </c>
       <c r="E45" s="8">
-        <v>612441</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
-      <c r="A46" s="12" t="s">
-        <v>340</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>341</v>
-      </c>
-      <c r="C46" s="5">
-        <v>352</v>
-      </c>
-      <c r="D46" s="5">
-        <v>339</v>
-      </c>
-      <c r="E46" s="8">
-        <v>611595</v>
+        <v>164616</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="21">
+      <c r="A46" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="C46" s="7">
+        <v>535</v>
+      </c>
+      <c r="D46" s="7">
+        <v>531</v>
+      </c>
+      <c r="E46" s="9">
+        <v>38344087</v>
       </c>
     </row>
     <row r="47" spans="1:5">
-      <c r="A47" s="12" t="s">
-        <v>310</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>311</v>
-      </c>
-      <c r="C47" s="9">
-        <v>1884</v>
-      </c>
-      <c r="D47" s="9">
-        <v>1884</v>
-      </c>
-      <c r="E47" s="9">
-        <v>568405</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="A48" s="12" t="s">
-        <v>283</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>284</v>
-      </c>
-      <c r="C48" s="9">
-        <v>3243</v>
-      </c>
-      <c r="D48" s="9">
-        <v>3209</v>
-      </c>
-      <c r="E48" s="8">
-        <v>506842</v>
+      <c r="A47" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="C47" s="7">
+        <v>523</v>
+      </c>
+      <c r="D47" s="7">
+        <v>522</v>
+      </c>
+      <c r="E47" s="8">
+        <v>5912447</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="21">
+      <c r="A48" s="13" t="s">
+        <v>320</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="C48" s="7">
+        <v>421</v>
+      </c>
+      <c r="D48" s="7">
+        <v>417</v>
+      </c>
+      <c r="E48" s="9">
+        <v>11973766</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="12" t="s">
-        <v>264</v>
+        <v>340</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>265</v>
+        <v>341</v>
       </c>
       <c r="C49" s="5">
-        <v>653</v>
+        <v>352</v>
       </c>
       <c r="D49" s="5">
-        <v>614</v>
+        <v>339</v>
       </c>
       <c r="E49" s="8">
-        <v>454533</v>
+        <v>611595</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -8268,75 +8270,75 @@
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="C51" s="7">
+        <v>273</v>
+      </c>
+      <c r="D51" s="7">
+        <v>281</v>
+      </c>
+      <c r="E51" s="8">
+        <v>10467235</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="21">
+      <c r="A52" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="C52" s="7">
+        <v>254</v>
+      </c>
+      <c r="D52" s="7">
+        <v>288</v>
+      </c>
+      <c r="E52" s="9">
+        <v>2822856</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="52.5">
+      <c r="A53" s="13" t="s">
+        <v>324</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>325</v>
+      </c>
+      <c r="C53" s="7">
+        <v>177</v>
+      </c>
+      <c r="D53" s="7">
+        <v>157</v>
+      </c>
+      <c r="E53" s="8">
+        <v>228901</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="13" t="s">
         <v>255</v>
       </c>
-      <c r="B51" s="6" t="s">
+      <c r="B54" s="6" t="s">
         <v>256</v>
       </c>
-      <c r="C51" s="7">
+      <c r="C54" s="7">
         <v>59</v>
       </c>
-      <c r="D51" s="7">
+      <c r="D54" s="7">
         <v>51</v>
       </c>
-      <c r="E51" s="9">
+      <c r="E54" s="9">
         <v>312989</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="52.5">
-      <c r="A52" s="13" t="s">
-        <v>324</v>
-      </c>
-      <c r="B52" s="6" t="s">
-        <v>325</v>
-      </c>
-      <c r="C52" s="7">
-        <v>177</v>
-      </c>
-      <c r="D52" s="7">
-        <v>157</v>
-      </c>
-      <c r="E52" s="8">
-        <v>228901</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="21">
-      <c r="A53" s="13" t="s">
-        <v>296</v>
-      </c>
-      <c r="B53" s="6" t="s">
-        <v>297</v>
-      </c>
-      <c r="C53" s="7">
-        <v>581</v>
-      </c>
-      <c r="D53" s="7">
-        <v>558</v>
-      </c>
-      <c r="E53" s="8">
-        <v>164616</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="21">
-      <c r="A54" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="C54" s="9">
-        <v>5000</v>
-      </c>
-      <c r="D54" s="9">
-        <v>5069</v>
-      </c>
-      <c r="E54" s="8">
-        <v>69472</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="A2:E54">
-    <sortCondition descending="1" ref="E1"/>
+    <sortCondition descending="1" ref="C1"/>
   </sortState>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>